<commit_message>
Generated Reports to be added
</commit_message>
<xml_diff>
--- a/data_files/final_dataset/calculated_performance.xlsx
+++ b/data_files/final_dataset/calculated_performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MD NADIM\Documents\NetBeansProjects\FindCochangeByClone\data_files\final_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123872AF-5E22-4FC6-A589-CC65C482740F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1686E2F5-898A-4E95-85FE-F02C5E7EA3DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>conqat</t>
   </si>
@@ -82,13 +82,64 @@
   </si>
   <si>
     <t>Changes</t>
+  </si>
+  <si>
+    <t>c1 to c10</t>
+  </si>
+  <si>
+    <t>c1, c3, c5, c6</t>
+  </si>
+  <si>
+    <t>c2, c3, c4, c6, c7</t>
+  </si>
+  <si>
+    <t>c1, c3, c4, c9</t>
+  </si>
+  <si>
+    <t>c1, c10</t>
+  </si>
+  <si>
+    <t>c1, c8, c9</t>
+  </si>
+  <si>
+    <t>c1, c2</t>
+  </si>
+  <si>
+    <t>4/10</t>
+  </si>
+  <si>
+    <t>5/10</t>
+  </si>
+  <si>
+    <t>2/10</t>
+  </si>
+  <si>
+    <t>3/10</t>
+  </si>
+  <si>
+    <t>Detection Accuracy</t>
+  </si>
+  <si>
+    <t>Changes at the same time</t>
+  </si>
+  <si>
+    <t>Cloned Cochnage</t>
+  </si>
+  <si>
+    <t>c1 to c20</t>
+  </si>
+  <si>
+    <t>Detected Cochange by Clone Detection Tools</t>
+  </si>
+  <si>
+    <t>Clone Detection Tools</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +158,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,12 +189,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -146,6 +200,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -179,6 +254,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Average Detection Accuracy</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -192,7 +293,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -840,7 +941,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$2</c15:sqref>
@@ -867,7 +968,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$3:$A$8</c15:sqref>
@@ -899,7 +1000,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$3:$C$8</c15:sqref>
@@ -930,7 +1031,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-1724-4D51-80DA-6CEFCB0E10BD}"/>
                   </c:ext>
@@ -1970,10 +2071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,17 +2097,17 @@
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2038,28 +2139,28 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>2103</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>13821</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.4</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.4</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.36</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>0.15</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>0.21</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>0.33</v>
       </c>
     </row>
@@ -2067,28 +2168,28 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>3299</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>69454</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.54</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.11</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>0.27</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>0.27</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>0.09</v>
       </c>
     </row>
@@ -2096,28 +2197,28 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>533</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>1963</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.23</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.12</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0.49</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>0.08</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>0.16</v>
       </c>
     </row>
@@ -2125,28 +2226,28 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>7514</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>246083</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.15</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.71</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0.09</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>0.11</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>0.06</v>
       </c>
     </row>
@@ -2154,28 +2255,28 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>6011</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>79417</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>0.16</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>0.69</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>0.11</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>0.15</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>0.15</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>0.09</v>
       </c>
     </row>
@@ -2183,28 +2284,28 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>3603</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>160689</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>0.11</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>0.74</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>0.06</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>0.19</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>0.1</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>0.04</v>
       </c>
     </row>
@@ -2238,7 +2339,7 @@
       <c r="D15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>3.36</v>
       </c>
     </row>
@@ -2246,50 +2347,174 @@
       <c r="D16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>1.34</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>1.25</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>0.92</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>0.83</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>0.77</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="D24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D29" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D15:E20">
     <sortCondition descending="1" ref="E15"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells count="10">
     <mergeCell ref="D1:I1"/>
+    <mergeCell ref="F25:F30"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="E25:E30"/>
+    <mergeCell ref="G24:I24"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started adding line coverage functionality
</commit_message>
<xml_diff>
--- a/data_files/final_dataset/calculated_performance.xlsx
+++ b/data_files/final_dataset/calculated_performance.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MD NADIM\Documents\NetBeansProjects\FindCochangeByClone\data_files\final_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1686E2F5-898A-4E95-85FE-F02C5E7EA3DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEA8515-61FD-4ABB-BD11-5CEC549E3CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>conqat</t>
   </si>
@@ -58,24 +59,6 @@
   </si>
   <si>
     <t>Detected Similar Cochange</t>
-  </si>
-  <si>
-    <t>brlcad</t>
-  </si>
-  <si>
-    <t>carol</t>
-  </si>
-  <si>
-    <t>ctags</t>
-  </si>
-  <si>
-    <t>freecol</t>
-  </si>
-  <si>
-    <t>jabref</t>
-  </si>
-  <si>
-    <t>jedit</t>
   </si>
   <si>
     <t>Total</t>
@@ -134,6 +117,45 @@
   <si>
     <t>Clone Detection Tools</t>
   </si>
+  <si>
+    <t>ConQAT</t>
+  </si>
+  <si>
+    <t>DECKARD</t>
+  </si>
+  <si>
+    <t>iClones</t>
+  </si>
+  <si>
+    <t>NiCad</t>
+  </si>
+  <si>
+    <t>SimCAD</t>
+  </si>
+  <si>
+    <t>Simian</t>
+  </si>
+  <si>
+    <t>BRLCAD</t>
+  </si>
+  <si>
+    <t>Carol</t>
+  </si>
+  <si>
+    <t>Ctags</t>
+  </si>
+  <si>
+    <t>Freecol</t>
+  </si>
+  <si>
+    <t>Jabref</t>
+  </si>
+  <si>
+    <t>jEdit</t>
+  </si>
+  <si>
+    <t>Average Number of Detected Clone by Revision</t>
+  </si>
 </sst>
 </file>
 
@@ -189,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -201,26 +223,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -260,7 +289,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="12000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -273,10 +302,17 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-CA" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
-              <a:t>Average Detection Accuracy</a:t>
+              <a:rPr lang="en-CA" b="1"/>
+              <a:t>Average Cloned</a:t>
             </a:r>
-            <a:endParaRPr lang="en-CA" b="1"/>
+            <a:r>
+              <a:rPr lang="en-CA" b="1" baseline="0"/>
+              <a:t> Cochange </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" b="1"/>
+              <a:t>Detection Accuracy</a:t>
+            </a:r>
           </a:p>
         </c:rich>
       </c:tx>
@@ -293,7 +329,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="12000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -325,7 +361,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>conqat</c:v>
+                  <c:v>ConQAT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -346,22 +382,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>brlcad</c:v>
+                  <c:v>BRLCAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>carol</c:v>
+                  <c:v>Carol</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ctags</c:v>
+                  <c:v>Ctags</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>freecol</c:v>
+                  <c:v>Freecol</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>jabref</c:v>
+                  <c:v>Jabref</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>jedit</c:v>
+                  <c:v>jEdit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -408,7 +444,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>deckard</c:v>
+                  <c:v>DECKARD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -429,22 +465,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>brlcad</c:v>
+                  <c:v>BRLCAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>carol</c:v>
+                  <c:v>Carol</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ctags</c:v>
+                  <c:v>Ctags</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>freecol</c:v>
+                  <c:v>Freecol</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>jabref</c:v>
+                  <c:v>Jabref</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>jedit</c:v>
+                  <c:v>jEdit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -491,7 +527,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>iclones</c:v>
+                  <c:v>iClones</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -512,22 +548,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>brlcad</c:v>
+                  <c:v>BRLCAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>carol</c:v>
+                  <c:v>Carol</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ctags</c:v>
+                  <c:v>Ctags</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>freecol</c:v>
+                  <c:v>Freecol</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>jabref</c:v>
+                  <c:v>Jabref</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>jedit</c:v>
+                  <c:v>jEdit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -574,7 +610,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>nicad5</c:v>
+                  <c:v>NiCad</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -595,22 +631,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>brlcad</c:v>
+                  <c:v>BRLCAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>carol</c:v>
+                  <c:v>Carol</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ctags</c:v>
+                  <c:v>Ctags</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>freecol</c:v>
+                  <c:v>Freecol</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>jabref</c:v>
+                  <c:v>Jabref</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>jedit</c:v>
+                  <c:v>jEdit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -657,7 +693,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>simcad</c:v>
+                  <c:v>SimCAD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -680,22 +716,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>brlcad</c:v>
+                  <c:v>BRLCAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>carol</c:v>
+                  <c:v>Carol</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ctags</c:v>
+                  <c:v>Ctags</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>freecol</c:v>
+                  <c:v>Freecol</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>jabref</c:v>
+                  <c:v>Jabref</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>jedit</c:v>
+                  <c:v>jEdit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -742,7 +778,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>simian</c:v>
+                  <c:v>Simian</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -765,22 +801,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>brlcad</c:v>
+                  <c:v>BRLCAD</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>carol</c:v>
+                  <c:v>Carol</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>ctags</c:v>
+                  <c:v>Ctags</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>freecol</c:v>
+                  <c:v>Freecol</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>jabref</c:v>
+                  <c:v>Jabref</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>jedit</c:v>
+                  <c:v>jEdit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -875,22 +911,22 @@
                     <c:strCache>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>brlcad</c:v>
+                        <c:v>BRLCAD</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>carol</c:v>
+                        <c:v>Carol</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>ctags</c:v>
+                        <c:v>Ctags</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>freecol</c:v>
+                        <c:v>Freecol</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>jabref</c:v>
+                        <c:v>Jabref</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>jedit</c:v>
+                        <c:v>jEdit</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -978,22 +1014,22 @@
                     <c:strCache>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>brlcad</c:v>
+                        <c:v>BRLCAD</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>carol</c:v>
+                        <c:v>Carol</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>ctags</c:v>
+                        <c:v>Ctags</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>freecol</c:v>
+                        <c:v>Freecol</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>jabref</c:v>
+                        <c:v>Jabref</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>jedit</c:v>
+                        <c:v>jEdit</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1070,7 +1106,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="10000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1129,6 +1165,720 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="10000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="588205344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="10000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="10000"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" b="1"/>
+              <a:t>Average Number of Detected</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" b="1" baseline="0"/>
+              <a:t> Clone by Revision</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ConQAT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1647.1775</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>622.67690000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>430.54590000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2624.6464000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1285.5345</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13018.981</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D0EE-46D4-8CA1-129A8D91DC14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DECKARD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3257.7557999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4118.5020999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>356.33640000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8516.0689000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6806.1857</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40076.729899999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D0EE-46D4-8CA1-129A8D91DC14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iClones</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>769.52059999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>226.63740000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.545900000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>690.1558</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>449.1515</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7648.2179999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D0EE-46D4-8CA1-129A8D91DC14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NiCad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$3:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>302.92380000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>233.28129999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>272.55579999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>412.64940000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>216.39189999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4068.3697000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D0EE-46D4-8CA1-129A8D91DC14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SimCAD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>841.48389999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>567.08529999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83.794899999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1173.4446</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>584.11469999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5338.4123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D0EE-46D4-8CA1-129A8D91DC14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$G$3:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>973.22990000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>244.90539999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>133.24469999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>624.19479999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>382.09559999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3132.1610999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D0EE-46D4-8CA1-129A8D91DC14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="427714016"/>
+        <c:axId val="427712704"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="427714016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -1144,7 +1894,66 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="588205344"/>
+        <c:crossAx val="427712704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="427712704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427714016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1264,6 +2073,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1767,20 +2616,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447674</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>100</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1788,6 +3140,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9173765-0EBB-4BBB-B3A2-7F8E22469595}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB716BA5-F17F-4666-B517-0FF8F2ECF5C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2073,8 +3466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,52 +3485,52 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4">
         <v>2103</v>
@@ -2166,7 +3559,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4">
         <v>3299</v>
@@ -2195,7 +3588,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4">
         <v>533</v>
@@ -2224,7 +3617,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4">
         <v>7514</v>
@@ -2253,7 +3646,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B7" s="4">
         <v>6011</v>
@@ -2282,7 +3675,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B8" s="4">
         <v>3603</v>
@@ -2384,116 +3777,116 @@
       </c>
     </row>
     <row r="24" spans="4:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="D24" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="6" t="s">
-        <v>28</v>
+      <c r="D24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="10" t="s">
-        <v>24</v>
+      <c r="G27" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="10" t="s">
-        <v>26</v>
+      <c r="G28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="10" t="s">
-        <v>27</v>
+      <c r="G29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="10" t="s">
-        <v>26</v>
+      <c r="G30" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2517,4 +3910,204 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C306F7-A961-4683-AD1F-B245EA0CD5D0}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1647.1775</v>
+      </c>
+      <c r="C3" s="12">
+        <v>3257.7557999999999</v>
+      </c>
+      <c r="D3" s="13">
+        <v>769.52059999999994</v>
+      </c>
+      <c r="E3" s="12">
+        <v>302.92380000000003</v>
+      </c>
+      <c r="F3" s="12">
+        <v>841.48389999999995</v>
+      </c>
+      <c r="G3" s="12">
+        <v>973.22990000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="12">
+        <v>622.67690000000005</v>
+      </c>
+      <c r="C4" s="12">
+        <v>4118.5020999999997</v>
+      </c>
+      <c r="D4" s="12">
+        <v>226.63740000000001</v>
+      </c>
+      <c r="E4" s="12">
+        <v>233.28129999999999</v>
+      </c>
+      <c r="F4" s="12">
+        <v>567.08529999999996</v>
+      </c>
+      <c r="G4" s="12">
+        <v>244.90539999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="12">
+        <v>430.54590000000002</v>
+      </c>
+      <c r="C5" s="12">
+        <v>356.33640000000003</v>
+      </c>
+      <c r="D5" s="12">
+        <v>88.545900000000003</v>
+      </c>
+      <c r="E5" s="12">
+        <v>272.55579999999998</v>
+      </c>
+      <c r="F5" s="12">
+        <v>83.794899999999998</v>
+      </c>
+      <c r="G5" s="12">
+        <v>133.24469999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2624.6464000000001</v>
+      </c>
+      <c r="C6" s="12">
+        <v>8516.0689000000002</v>
+      </c>
+      <c r="D6" s="12">
+        <v>690.1558</v>
+      </c>
+      <c r="E6" s="12">
+        <v>412.64940000000001</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1173.4446</v>
+      </c>
+      <c r="G6" s="12">
+        <v>624.19479999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1285.5345</v>
+      </c>
+      <c r="C7" s="12">
+        <v>6806.1857</v>
+      </c>
+      <c r="D7" s="12">
+        <v>449.1515</v>
+      </c>
+      <c r="E7" s="12">
+        <v>216.39189999999999</v>
+      </c>
+      <c r="F7" s="12">
+        <v>584.11469999999997</v>
+      </c>
+      <c r="G7" s="12">
+        <v>382.09559999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="12">
+        <v>13018.981</v>
+      </c>
+      <c r="C8" s="12">
+        <v>40076.729899999998</v>
+      </c>
+      <c r="D8" s="12">
+        <v>7648.2179999999998</v>
+      </c>
+      <c r="E8" s="12">
+        <v>4068.3697000000002</v>
+      </c>
+      <c r="F8" s="12">
+        <v>5338.4123</v>
+      </c>
+      <c r="G8" s="12">
+        <v>3132.1610999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Line Coverage and it's average
</commit_message>
<xml_diff>
--- a/data_files/final_dataset/calculated_performance.xlsx
+++ b/data_files/final_dataset/calculated_performance.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MD NADIM\Documents\NetBeansProjects\FindCochangeByClone\data_files\final_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEA8515-61FD-4ABB-BD11-5CEC549E3CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B88AD8-6C85-44EE-9F31-C69B9A70B45D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
+    <sheet name="Clone fragments by revision" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
   <si>
     <t>conqat</t>
   </si>
@@ -211,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -232,6 +232,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -244,10 +254,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,7 +363,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Accuracy!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -378,7 +384,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Accuracy!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -404,7 +410,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$8</c:f>
+              <c:f>Accuracy!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -440,7 +446,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Accuracy!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -461,7 +467,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Accuracy!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -487,7 +493,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$8</c:f>
+              <c:f>Accuracy!$E$3:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -523,7 +529,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
+              <c:f>Accuracy!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -544,7 +550,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Accuracy!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -570,7 +576,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$8</c:f>
+              <c:f>Accuracy!$F$3:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -606,7 +612,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Accuracy!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -627,7 +633,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Accuracy!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -653,7 +659,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$8</c:f>
+              <c:f>Accuracy!$G$3:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -689,7 +695,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
+              <c:f>Accuracy!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -712,7 +718,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Accuracy!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -738,7 +744,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$8</c:f>
+              <c:f>Accuracy!$H$3:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -774,7 +780,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$2</c:f>
+              <c:f>Accuracy!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -797,7 +803,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Accuracy!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -823,7 +829,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$8</c:f>
+              <c:f>Accuracy!$I$3:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -877,7 +883,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$2</c15:sqref>
+                          <c15:sqref>Accuracy!$B$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -904,7 +910,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$3:$A$8</c15:sqref>
+                          <c15:sqref>Accuracy!$A$3:$A$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -936,7 +942,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$3:$B$8</c15:sqref>
+                          <c15:sqref>Accuracy!$B$3:$B$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -980,7 +986,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$2</c15:sqref>
+                          <c15:sqref>Accuracy!$C$2</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1007,7 +1013,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$3:$A$8</c15:sqref>
+                          <c15:sqref>Accuracy!$A$3:$A$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1039,7 +1045,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$C$3:$C$8</c15:sqref>
+                          <c15:sqref>Accuracy!$C$3:$C$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1345,7 +1351,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$2</c:f>
+              <c:f>'Clone fragments by revision'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1366,7 +1372,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:f>'Clone fragments by revision'!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1392,7 +1398,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$3:$B$8</c:f>
+              <c:f>'Clone fragments by revision'!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1428,7 +1434,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$2</c:f>
+              <c:f>'Clone fragments by revision'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1449,7 +1455,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:f>'Clone fragments by revision'!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1475,7 +1481,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$3:$C$8</c:f>
+              <c:f>'Clone fragments by revision'!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1511,7 +1517,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$2</c:f>
+              <c:f>'Clone fragments by revision'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1532,7 +1538,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:f>'Clone fragments by revision'!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1558,7 +1564,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$3:$D$8</c:f>
+              <c:f>'Clone fragments by revision'!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1594,7 +1600,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$E$2</c:f>
+              <c:f>'Clone fragments by revision'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1615,7 +1621,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:f>'Clone fragments by revision'!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1641,7 +1647,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$E$3:$E$8</c:f>
+              <c:f>'Clone fragments by revision'!$E$3:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1677,7 +1683,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$F$2</c:f>
+              <c:f>'Clone fragments by revision'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1698,7 +1704,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:f>'Clone fragments by revision'!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1724,7 +1730,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$F$3:$F$8</c:f>
+              <c:f>'Clone fragments by revision'!$F$3:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1760,7 +1766,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$G$2</c:f>
+              <c:f>'Clone fragments by revision'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1781,7 +1787,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$3:$A$8</c:f>
+              <c:f>'Clone fragments by revision'!$A$3:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1807,7 +1813,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$G$3:$G$8</c:f>
+              <c:f>'Clone fragments by revision'!$G$3:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3170,10 +3176,10 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3464,10 +3470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I8"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3490,14 +3496,14 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -3786,11 +3792,11 @@
       <c r="F24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="5" t="s">
         <v>22</v>
       </c>
@@ -3799,17 +3805,17 @@
       <c r="D25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
       <c r="J25" s="7" t="s">
         <v>18</v>
       </c>
@@ -3818,13 +3824,13 @@
       <c r="D26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="10" t="s">
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
       <c r="J26" s="7" t="s">
         <v>19</v>
       </c>
@@ -3833,13 +3839,13 @@
       <c r="D27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="10" t="s">
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
       <c r="J27" s="7" t="s">
         <v>18</v>
       </c>
@@ -3848,13 +3854,13 @@
       <c r="D28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="10" t="s">
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
       <c r="J28" s="7" t="s">
         <v>20</v>
       </c>
@@ -3863,13 +3869,13 @@
       <c r="D29" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="10" t="s">
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
       <c r="J29" s="7" t="s">
         <v>21</v>
       </c>
@@ -3878,22 +3884,194 @@
       <c r="D30" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="10" t="s">
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
       <c r="J30" s="7" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.36</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.54</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.71</v>
+      </c>
+      <c r="D44" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="G44" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="E46" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D15:E20">
     <sortCondition descending="1" ref="E15"/>
   </sortState>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B39:G39"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="F25:F30"/>
     <mergeCell ref="G25:I25"/>
@@ -3914,10 +4092,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C306F7-A961-4683-AD1F-B245EA0CD5D0}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3926,20 +4104,19 @@
     <col min="2" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -3968,22 +4145,22 @@
       <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="8">
         <v>1647.1775</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="8">
         <v>3257.7557999999999</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="9">
         <v>769.52059999999994</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="8">
         <v>302.92380000000003</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="8">
         <v>841.48389999999995</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="8">
         <v>973.22990000000004</v>
       </c>
     </row>
@@ -3991,22 +4168,22 @@
       <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="8">
         <v>622.67690000000005</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="8">
         <v>4118.5020999999997</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="8">
         <v>226.63740000000001</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="8">
         <v>233.28129999999999</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="8">
         <v>567.08529999999996</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="8">
         <v>244.90539999999999</v>
       </c>
     </row>
@@ -4014,22 +4191,22 @@
       <c r="A5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="8">
         <v>430.54590000000002</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="8">
         <v>356.33640000000003</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="8">
         <v>88.545900000000003</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="8">
         <v>272.55579999999998</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="8">
         <v>83.794899999999998</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="8">
         <v>133.24469999999999</v>
       </c>
     </row>
@@ -4037,22 +4214,22 @@
       <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="8">
         <v>2624.6464000000001</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="8">
         <v>8516.0689000000002</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="8">
         <v>690.1558</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="8">
         <v>412.64940000000001</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="8">
         <v>1173.4446</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="8">
         <v>624.19479999999999</v>
       </c>
     </row>
@@ -4060,22 +4237,22 @@
       <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="8">
         <v>1285.5345</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="8">
         <v>6806.1857</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="8">
         <v>449.1515</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="8">
         <v>216.39189999999999</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="8">
         <v>584.11469999999997</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="8">
         <v>382.09559999999999</v>
       </c>
     </row>
@@ -4083,24 +4260,205 @@
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="8">
         <v>13018.981</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="8">
         <v>40076.729899999998</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="8">
         <v>7648.2179999999998</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="8">
         <v>4068.3697000000002</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="8">
         <v>5338.4123</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="8">
         <v>3132.1610999999998</v>
       </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1647.1775</v>
+      </c>
+      <c r="C19" s="8">
+        <v>622.67690000000005</v>
+      </c>
+      <c r="D19" s="8">
+        <v>430.54590000000002</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2624.6464000000001</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1285.5345</v>
+      </c>
+      <c r="G19" s="8">
+        <v>13018.981</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3257.7557999999999</v>
+      </c>
+      <c r="C20" s="8">
+        <v>4118.5020999999997</v>
+      </c>
+      <c r="D20" s="8">
+        <v>356.33640000000003</v>
+      </c>
+      <c r="E20" s="8">
+        <v>8516.0689000000002</v>
+      </c>
+      <c r="F20" s="8">
+        <v>6806.1857</v>
+      </c>
+      <c r="G20" s="8">
+        <v>40076.729899999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="9">
+        <v>769.52059999999994</v>
+      </c>
+      <c r="C21" s="8">
+        <v>226.63740000000001</v>
+      </c>
+      <c r="D21" s="8">
+        <v>88.545900000000003</v>
+      </c>
+      <c r="E21" s="8">
+        <v>690.1558</v>
+      </c>
+      <c r="F21" s="8">
+        <v>449.1515</v>
+      </c>
+      <c r="G21" s="8">
+        <v>7648.2179999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="8">
+        <v>302.92380000000003</v>
+      </c>
+      <c r="C22" s="8">
+        <v>233.28129999999999</v>
+      </c>
+      <c r="D22" s="8">
+        <v>272.55579999999998</v>
+      </c>
+      <c r="E22" s="8">
+        <v>412.64940000000001</v>
+      </c>
+      <c r="F22" s="8">
+        <v>216.39189999999999</v>
+      </c>
+      <c r="G22" s="8">
+        <v>4068.3697000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="8">
+        <v>841.48389999999995</v>
+      </c>
+      <c r="C23" s="8">
+        <v>567.08529999999996</v>
+      </c>
+      <c r="D23" s="8">
+        <v>83.794899999999998</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1173.4446</v>
+      </c>
+      <c r="F23" s="8">
+        <v>584.11469999999997</v>
+      </c>
+      <c r="G23" s="8">
+        <v>5338.4123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="8">
+        <v>973.22990000000004</v>
+      </c>
+      <c r="C24" s="8">
+        <v>244.90539999999999</v>
+      </c>
+      <c r="D24" s="8">
+        <v>133.24469999999999</v>
+      </c>
+      <c r="E24" s="8">
+        <v>624.19479999999999</v>
+      </c>
+      <c r="F24" s="8">
+        <v>382.09559999999999</v>
+      </c>
+      <c r="G24" s="8">
+        <v>3132.1610999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Calculated recall for merged tool combination
</commit_message>
<xml_diff>
--- a/data_files/final_dataset/calculated_performance.xlsx
+++ b/data_files/final_dataset/calculated_performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_USASK\Programming@USASK\FindCochangeByClone\data_files\final_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9409A6-C0CF-4112-A757-37FA1E0E3480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219D2134-20C1-41AA-A59D-BA4D3A805378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="avg_precision" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="65">
   <si>
     <t>conqat</t>
   </si>
@@ -226,6 +228,12 @@
   <si>
     <t>Category  of Information</t>
   </si>
+  <si>
+    <t>Deckard</t>
+  </si>
+  <si>
+    <t>Number of Changes</t>
+  </si>
 </sst>
 </file>
 
@@ -317,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -389,18 +397,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -419,14 +415,29 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1464,15 +1475,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA" b="1"/>
-              <a:t>Average Cloned</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" b="1" baseline="0"/>
-              <a:t> Cochange </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" b="1"/>
-              <a:t>Detection Accuracy</a:t>
+              <a:t>Average Recall</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1593,89 +1596,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-1724-4D51-80DA-6CEFCB0E10BD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Recall!$E$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DECKARD</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Recall!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>BRLCAD</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Carol</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Ctags</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Freecol</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Jabref</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>jEdit</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Recall!$E$3:$E$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.54</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.28000000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.71</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.74</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-1724-4D51-80DA-6CEFCB0E10BD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2231,6 +2151,109 @@
                 <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-1724-4D51-80DA-6CEFCB0E10BD}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Recall!$E$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Deckard</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Recall!$A$3:$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>BRLCAD</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Carol</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Ctags</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Freecol</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Jabref</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>jEdit</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Recall!$E$3:$E$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>0.4</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.54</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.28000000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.71</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.69</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.74</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-1724-4D51-80DA-6CEFCB0E10BD}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -4231,6 +4254,1420 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average F1 Score in Each Subject System</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'f1-score'!$X$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ConQAT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'f1-score'!$U$3:$U$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'f1-score'!$X$3:$X$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.41688950288731225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24599459864556097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22870485782322589</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16600151805391328</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1977906195755415</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10711881551627447</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-57EF-40F4-B191-4B201A50A322}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'f1-score'!$Y$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DECKARD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'f1-score'!$U$3:$U$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'f1-score'!$Y$3:$Y$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.27910826982035358</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31453517916582213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20193101124985169</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29537217322503428</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.20234800581108553</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11663137705496668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-57EF-40F4-B191-4B201A50A322}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'f1-score'!$Z$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iClones</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'f1-score'!$U$3:$U$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'f1-score'!$Z$3:$Z$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.37994793582493364</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14855926804305797</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12710982332687351</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1002228851511482E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14408274466351104</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.2204563575822915E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-57EF-40F4-B191-4B201A50A322}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'f1-score'!$AA$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NiCad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'f1-score'!$U$3:$U$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'f1-score'!$AA$3:$AA$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.18720052585610855</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30129494838224291</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31382654030624113</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2868115404567603E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17475320466887764</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.14448929846874659</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-57EF-40F4-B191-4B201A50A322}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'f1-score'!$AB$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SimCAD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'f1-score'!$U$3:$U$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'f1-score'!$AB$3:$AB$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.25460484763440394</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30399255828716093</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4889193309519477E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12020512383183293</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17958363875605404</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.8944786679593504E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-57EF-40F4-B191-4B201A50A322}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'f1-score'!$AC$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'f1-score'!$U$3:$U$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>BRLCAD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carol</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Ctags</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Freecol</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jabref</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jEdit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'f1-score'!$AC$3:$AC$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.35925383467930827</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12836136424048061</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16656442463127666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1133273679729644E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12063872076882967</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9880204159506149E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-57EF-40F4-B191-4B201A50A322}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="412814591"/>
+        <c:axId val="936923599"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'f1-score'!$V$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Changes</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'f1-score'!$U$3:$U$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>BRLCAD</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Carol</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Ctags</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Freecol</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Jabref</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>jEdit</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'f1-score'!$V$3:$V$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>2103</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3299</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>533</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>7514</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>6011</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>3603</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-57EF-40F4-B191-4B201A50A322}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'f1-score'!$W$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Similar Cochange</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'f1-score'!$U$3:$U$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>BRLCAD</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Carol</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Ctags</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Freecol</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Jabref</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>jEdit</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'f1-score'!$W$3:$W$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>13821</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>69454</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1963</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>246083</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>79417</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>160689</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-57EF-40F4-B191-4B201A50A322}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="412814591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="936923599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="936923599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="412814591"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1500"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4431,6 +5868,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6946,6 +8423,530 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -7141,6 +9142,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>201707</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85164</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>753035</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>8963</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{554BB2C9-536C-4CD2-8E41-375E4CAE2972}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7439,14 +9481,14 @@
       <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -7735,11 +9777,11 @@
       <c r="F24" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="28" t="s">
+      <c r="G24" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
       <c r="J24" s="13" t="s">
         <v>22</v>
       </c>
@@ -7748,17 +9790,17 @@
       <c r="D25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G25" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
       <c r="J25" s="7" t="s">
         <v>18</v>
       </c>
@@ -7767,13 +9809,13 @@
       <c r="D26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="30" t="s">
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
       <c r="J26" s="7" t="s">
         <v>19</v>
       </c>
@@ -7782,13 +9824,13 @@
       <c r="D27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="30" t="s">
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
       <c r="J27" s="7" t="s">
         <v>18</v>
       </c>
@@ -7797,13 +9839,13 @@
       <c r="D28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30" t="s">
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
       <c r="J28" s="7" t="s">
         <v>20</v>
       </c>
@@ -7812,13 +9854,13 @@
       <c r="D29" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30" t="s">
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
       <c r="J29" s="7" t="s">
         <v>21</v>
       </c>
@@ -7827,26 +9869,26 @@
       <c r="D30" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30" t="s">
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
       <c r="J30" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
@@ -8033,8 +10075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:I9"/>
+    <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="EV219" sqref="EV219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8058,14 +10100,14 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -8080,8 +10122,8 @@
       <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
+      <c r="E2" s="27" t="s">
+        <v>63</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>30</v>
@@ -8354,11 +10396,11 @@
       <c r="F24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="28" t="s">
+      <c r="G24" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
       <c r="J24" s="5" t="s">
         <v>22</v>
       </c>
@@ -8367,17 +10409,17 @@
       <c r="D25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G25" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
       <c r="J25" s="7" t="s">
         <v>18</v>
       </c>
@@ -8386,13 +10428,13 @@
       <c r="D26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="30" t="s">
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
       <c r="J26" s="7" t="s">
         <v>19</v>
       </c>
@@ -8401,13 +10443,13 @@
       <c r="D27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="30" t="s">
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
       <c r="J27" s="7" t="s">
         <v>18</v>
       </c>
@@ -8416,13 +10458,13 @@
       <c r="D28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30" t="s">
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
       <c r="J28" s="7" t="s">
         <v>20</v>
       </c>
@@ -8431,13 +10473,13 @@
       <c r="D29" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30" t="s">
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
       <c r="J29" s="7" t="s">
         <v>21</v>
       </c>
@@ -8446,26 +10488,26 @@
       <c r="D30" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30" t="s">
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
       <c r="J30" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
@@ -8474,8 +10516,8 @@
       <c r="B40" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>29</v>
+      <c r="C40" s="27" t="s">
+        <v>63</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>30</v>
@@ -8656,7 +10698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C306F7-A961-4683-AD1F-B245EA0CD5D0}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G39" sqref="G39:Q41"/>
     </sheetView>
   </sheetViews>
@@ -8673,16 +10715,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -8916,30 +10958,30 @@
       <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="28">
         <v>13470.63</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="28">
         <v>15276.22</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="28">
         <v>11239.19</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="28">
         <v>9874.83</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="28">
         <v>11604.93</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="28">
         <v>13433.31</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -8964,10 +11006,10 @@
       <c r="H18" t="s">
         <v>39</v>
       </c>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
@@ -8992,10 +11034,10 @@
       <c r="H19" s="8">
         <v>13018.981</v>
       </c>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -9149,167 +11191,167 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="36">
+      <c r="E31" s="32">
         <v>5792.4970000000003</v>
       </c>
-      <c r="H31" s="33" t="s">
+      <c r="H31" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="35">
+      <c r="I31" s="31">
         <v>15276.22</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="32">
         <v>1747.3693000000001</v>
       </c>
-      <c r="H32" s="33" t="s">
+      <c r="H32" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="35">
+      <c r="I32" s="31">
         <v>13470.63</v>
       </c>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="32">
         <v>838.33299999999997</v>
       </c>
-      <c r="H33" s="33" t="s">
+      <c r="H33" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="I33" s="35">
+      <c r="I33" s="31">
         <v>13433.3</v>
       </c>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="32">
         <v>728</v>
       </c>
-      <c r="H34" s="33" t="s">
+      <c r="H34" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="I34" s="35">
+      <c r="I34" s="31">
         <v>11604.9</v>
       </c>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="32">
         <v>634.61699999999996</v>
       </c>
-      <c r="H35" s="33" t="s">
+      <c r="H35" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="35">
+      <c r="I35" s="31">
         <v>11239</v>
       </c>
     </row>
     <row r="36" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="36">
+      <c r="E36" s="32">
         <v>400.83</v>
       </c>
-      <c r="H36" s="33" t="s">
+      <c r="H36" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="35">
+      <c r="I36" s="31">
         <v>9874.7999999999993</v>
       </c>
     </row>
     <row r="39" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="G39" s="37" t="s">
+      <c r="G39" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="38" t="s">
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="M39" s="38" t="s">
+      <c r="M39" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="N39" s="38" t="s">
+      <c r="N39" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="O39" s="38" t="s">
+      <c r="O39" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="P39" s="38" t="s">
+      <c r="P39" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="Q39" s="38" t="s">
+      <c r="Q39" s="33" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="40" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="G40" s="37" t="s">
+      <c r="G40" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="37"/>
-      <c r="L40" s="39">
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="34">
         <v>5792.4970000000003</v>
       </c>
-      <c r="M40" s="39">
+      <c r="M40" s="34">
         <v>1747.3693000000001</v>
       </c>
-      <c r="N40" s="39">
+      <c r="N40" s="34">
         <v>838.33299999999997</v>
       </c>
-      <c r="O40" s="39">
+      <c r="O40" s="34">
         <v>728</v>
       </c>
-      <c r="P40" s="39">
+      <c r="P40" s="34">
         <v>634.61699999999996</v>
       </c>
-      <c r="Q40" s="39">
+      <c r="Q40" s="34">
         <v>400.83</v>
       </c>
     </row>
     <row r="41" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="G41" s="37" t="s">
+      <c r="G41" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="37"/>
-      <c r="L41" s="39">
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="34">
         <v>15276.22</v>
       </c>
-      <c r="M41" s="39">
+      <c r="M41" s="34">
         <v>13470.63</v>
       </c>
-      <c r="N41" s="39">
+      <c r="N41" s="34">
         <v>13433.3</v>
       </c>
-      <c r="O41" s="39">
+      <c r="O41" s="34">
         <v>11604.9</v>
       </c>
-      <c r="P41" s="39">
+      <c r="P41" s="34">
         <v>11239</v>
       </c>
-      <c r="Q41" s="39">
+      <c r="Q41" s="34">
         <v>9874.7999999999993</v>
       </c>
     </row>
@@ -9333,8 +11375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1BD61D-A86A-42A4-92F7-17736722A0D0}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18:X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9375,42 +11417,42 @@
       <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="L1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
       <c r="V1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="W1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="X1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -10079,43 +12121,93 @@
         <v>0.77000000000000013</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X18" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W19" t="s">
+        <v>34</v>
+      </c>
+      <c r="X19" s="4">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="W20" t="s">
+        <v>35</v>
+      </c>
+      <c r="X20" s="4">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="W21" t="s">
+        <v>36</v>
+      </c>
+      <c r="X21" s="4">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="W22" t="s">
+        <v>37</v>
+      </c>
+      <c r="X22" s="4">
+        <v>7514</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="W23" t="s">
+        <v>38</v>
+      </c>
+      <c r="X23" s="4">
+        <v>6011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="W24" t="s">
+        <v>39</v>
+      </c>
+      <c r="X24" s="4">
+        <v>3603</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="W19:X24">
+    <sortCondition ref="W19"/>
+  </sortState>
   <mergeCells count="3">
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="N1:S1"/>
     <mergeCell ref="X1:AC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10124,7 +12216,7 @@
   <dimension ref="A1:AC39"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B8"/>
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10165,42 +12257,42 @@
       <c r="C1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="L1" s="16" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
       <c r="V1" s="16" t="s">
         <v>9</v>
       </c>
       <c r="W1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="X1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">

</xml_diff>